<commit_message>
ZwaerteVallei works with Newton on and is fast.
</commit_message>
<xml_diff>
--- a/Projects/VoortoetsAGT/cases/Dijlevallei/DijleVallei.xlsx
+++ b/Projects/VoortoetsAGT/cases/Dijlevallei/DijleVallei.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Theo/GRWMODELS/python/mf6lab/Projects/VoortoetsAGT/cases/MoervaarDpr/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Theo/GRWMODELS/python/mf6lab/Projects/VoortoetsAGT/cases/Dijlevallei/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C48887F3-6AA6-5C4A-AFFC-199370999FCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3F7FC60-5930-3548-AAB5-4538DF86BBA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7320" yWindow="-19860" windowWidth="30600" windowHeight="19860" tabRatio="751" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-3720" yWindow="-22980" windowWidth="26540" windowHeight="15980" tabRatio="751" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NAM" sheetId="1" r:id="rId1"/>
@@ -205,7 +205,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2499" uniqueCount="420">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2505" uniqueCount="418">
   <si>
     <t>ON / OFF</t>
   </si>
@@ -1371,9 +1371,6 @@
     <t>SIMPLE | MODERATE | COMPLEX</t>
   </si>
   <si>
-    <t>SIMPLE</t>
-  </si>
-  <si>
     <t>METER</t>
   </si>
   <si>
@@ -1398,42 +1395,9 @@
     <t>Eolisch deklagen buiten Roerdalslenk</t>
   </si>
   <si>
-    <t>A0170</t>
-  </si>
-  <si>
     <t>Pleisocene afzettingen</t>
   </si>
   <si>
-    <t>A0430</t>
-  </si>
-  <si>
-    <t>Runsbroek-Berg Aquifer</t>
-  </si>
-  <si>
-    <t>A0440</t>
-  </si>
-  <si>
-    <t>Tongeren Aquitard</t>
-  </si>
-  <si>
-    <t>A0450</t>
-  </si>
-  <si>
-    <t>Onder Oligoceen Aquifersysteem</t>
-  </si>
-  <si>
-    <t>A0500</t>
-  </si>
-  <si>
-    <t>Bartoon Aquitardsysteem</t>
-  </si>
-  <si>
-    <t>A0610</t>
-  </si>
-  <si>
-    <t>Wemmel Lede Aquifer</t>
-  </si>
-  <si>
     <t>Sy</t>
   </si>
   <si>
@@ -1449,12 +1413,6 @@
     <t>orange</t>
   </si>
   <si>
-    <t>gold</t>
-  </si>
-  <si>
-    <t>lightskyblue</t>
-  </si>
-  <si>
     <t>lightsalmon</t>
   </si>
   <si>
@@ -1465,6 +1423,42 @@
   </si>
   <si>
     <t>yellowgreen</t>
+  </si>
+  <si>
+    <t>A0???</t>
+  </si>
+  <si>
+    <t>Paarse laag</t>
+  </si>
+  <si>
+    <t>Grijsgroene laag</t>
+  </si>
+  <si>
+    <t>lightyellow</t>
+  </si>
+  <si>
+    <t>green</t>
+  </si>
+  <si>
+    <t>darkgreen</t>
+  </si>
+  <si>
+    <t>Violette laag</t>
+  </si>
+  <si>
+    <t>Zalmkleurige laag</t>
+  </si>
+  <si>
+    <t>Bruine laag</t>
+  </si>
+  <si>
+    <t>Groene laag</t>
+  </si>
+  <si>
+    <t>Donker groene laag</t>
+  </si>
+  <si>
+    <t>darkviolet</t>
   </si>
 </sst>
 </file>
@@ -2745,7 +2739,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9985BC8C-AF94-474C-A200-72B17F25D172}">
   <dimension ref="A1:C115"/>
   <sheetViews>
-    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+    <sheetView topLeftCell="A30" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
@@ -3579,8 +3573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C06500DB-BECE-8C4B-B4E6-A47BC546FCEB}">
   <dimension ref="A1:H477"/>
   <sheetViews>
-    <sheetView topLeftCell="A107" zoomScale="182" zoomScaleNormal="182" workbookViewId="0">
-      <selection activeCell="C324" sqref="C324"/>
+    <sheetView tabSelected="1" zoomScale="182" zoomScaleNormal="182" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3705,7 +3699,7 @@
         <v>114</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="D11" s="11" t="s">
         <v>387</v>
@@ -4335,7 +4329,7 @@
         <v>51</v>
       </c>
       <c r="C71" s="11" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.15">
@@ -12588,10 +12582,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:I55"/>
+  <dimension ref="A1:I57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="237" zoomScaleNormal="237" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView zoomScale="237" zoomScaleNormal="237" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -12604,7 +12598,7 @@
         <v>13</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>79</v>
@@ -12613,19 +12607,19 @@
         <v>81</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>409</v>
+        <v>397</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>410</v>
+        <v>398</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>411</v>
+        <v>399</v>
       </c>
       <c r="H1" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>391</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>392</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.15">
@@ -12648,13 +12642,13 @@
         <v>1E-4</v>
       </c>
       <c r="G2" s="16" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="H2" s="11" t="s">
+        <v>392</v>
+      </c>
+      <c r="I2" s="11" t="s">
         <v>393</v>
-      </c>
-      <c r="I2" s="11" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.15">
@@ -12677,13 +12671,13 @@
         <v>1E-4</v>
       </c>
       <c r="G3" s="16" t="s">
-        <v>413</v>
+        <v>401</v>
       </c>
       <c r="H3" s="11" t="s">
+        <v>394</v>
+      </c>
+      <c r="I3" s="11" t="s">
         <v>395</v>
-      </c>
-      <c r="I3" s="11" t="s">
-        <v>396</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.15">
@@ -12694,25 +12688,25 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>50</v>
+        <v>0.5</v>
       </c>
       <c r="D4">
-        <v>25</v>
+        <v>0.2</v>
       </c>
       <c r="E4">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
       <c r="F4" s="2">
         <v>1E-4</v>
       </c>
       <c r="G4" s="16" t="s">
-        <v>414</v>
+        <v>403</v>
       </c>
       <c r="H4" s="11" t="s">
-        <v>397</v>
+        <v>406</v>
       </c>
       <c r="I4" s="11" t="s">
-        <v>398</v>
+        <v>407</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.15">
@@ -12720,13 +12714,13 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5">
-        <v>10</v>
+        <v>0.1</v>
       </c>
       <c r="D5">
-        <v>2</v>
+        <v>0.02</v>
       </c>
       <c r="E5">
         <v>0.1</v>
@@ -12735,13 +12729,13 @@
         <v>1E-4</v>
       </c>
       <c r="G5" s="16" t="s">
-        <v>415</v>
+        <v>405</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>399</v>
+        <v>406</v>
       </c>
       <c r="I5" s="11" t="s">
-        <v>400</v>
+        <v>408</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.15">
@@ -12749,28 +12743,28 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6" s="2">
-        <v>1E-3</v>
-      </c>
-      <c r="D6" s="2">
-        <v>1E-3</v>
-      </c>
-      <c r="E6" s="2">
-        <v>0.1</v>
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>50</v>
+      </c>
+      <c r="D6">
+        <v>25</v>
+      </c>
+      <c r="E6">
+        <v>0.25</v>
       </c>
       <c r="F6" s="2">
         <v>1E-4</v>
       </c>
       <c r="G6" s="16" t="s">
-        <v>416</v>
+        <v>400</v>
       </c>
       <c r="H6" s="11" t="s">
-        <v>401</v>
+        <v>406</v>
       </c>
       <c r="I6" s="11" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.15">
@@ -12781,10 +12775,10 @@
         <v>0</v>
       </c>
       <c r="C7">
-        <v>2</v>
+        <v>0.1</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>0.03</v>
       </c>
       <c r="E7">
         <v>0.1</v>
@@ -12796,10 +12790,10 @@
         <v>417</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>403</v>
+        <v>406</v>
       </c>
       <c r="I7" s="11" t="s">
-        <v>404</v>
+        <v>412</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.15">
@@ -12810,10 +12804,10 @@
         <v>0</v>
       </c>
       <c r="C8" s="2">
-        <v>1E-3</v>
+        <v>3</v>
       </c>
       <c r="D8" s="2">
-        <v>1E-3</v>
+        <v>1</v>
       </c>
       <c r="E8" s="2">
         <v>0.1</v>
@@ -12822,13 +12816,13 @@
         <v>1E-4</v>
       </c>
       <c r="G8" s="16" t="s">
-        <v>418</v>
+        <v>402</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="I8" s="11" t="s">
-        <v>406</v>
+        <v>413</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.15">
@@ -12839,10 +12833,10 @@
         <v>0</v>
       </c>
       <c r="C9">
-        <v>5</v>
+        <v>0.01</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="E9">
         <v>0.1</v>
@@ -12851,26 +12845,72 @@
         <v>1E-4</v>
       </c>
       <c r="G9" s="16" t="s">
-        <v>419</v>
+        <v>404</v>
       </c>
       <c r="H9" s="11" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="I9" s="11" t="s">
-        <v>408</v>
+        <v>414</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="D10" s="2">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="F10" s="2">
+        <v>1E-4</v>
+      </c>
+      <c r="G10" s="16" t="s">
+        <v>410</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>406</v>
+      </c>
+      <c r="I10" s="11" t="s">
+        <v>415</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>1E-4</v>
+      </c>
+      <c r="D11">
+        <v>3.0000000000000001E-5</v>
+      </c>
+      <c r="E11">
+        <v>0.1</v>
+      </c>
+      <c r="F11" s="2">
+        <v>1E-4</v>
+      </c>
+      <c r="G11" s="16" t="s">
+        <v>411</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>406</v>
+      </c>
+      <c r="I11" s="11" t="s">
+        <v>416</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.15">
       <c r="D12" s="2"/>
@@ -13135,6 +13175,18 @@
       <c r="E55" s="2"/>
       <c r="F55" s="2"/>
       <c r="G55" s="2"/>
+    </row>
+    <row r="56" spans="4:7" x14ac:dyDescent="0.15">
+      <c r="D56" s="2"/>
+      <c r="E56" s="2"/>
+      <c r="F56" s="2"/>
+      <c r="G56" s="2"/>
+    </row>
+    <row r="57" spans="4:7" x14ac:dyDescent="0.15">
+      <c r="D57" s="2"/>
+      <c r="E57" s="2"/>
+      <c r="F57" s="2"/>
+      <c r="G57" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
DijleVallei adapted with correct layeres, according to David Simpson.
</commit_message>
<xml_diff>
--- a/Projects/VoortoetsAGT/cases/Dijlevallei/DijleVallei.xlsx
+++ b/Projects/VoortoetsAGT/cases/Dijlevallei/DijleVallei.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Theo/GRWMODELS/python/mf6lab/Projects/VoortoetsAGT/cases/Dijlevallei/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD7BFBE2-9008-944B-809D-0696F291109A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4AB2E24-CD4B-FE47-908C-18B189885857}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3720" yWindow="-22980" windowWidth="26540" windowHeight="15980" tabRatio="751" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-3720" yWindow="-22980" windowWidth="26540" windowHeight="15980" tabRatio="751" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NAM" sheetId="1" r:id="rId1"/>
@@ -205,7 +205,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2500" uniqueCount="416">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2503" uniqueCount="427">
   <si>
     <t>ON / OFF</t>
   </si>
@@ -1383,9 +1383,6 @@
     <t>Eolisch deklagen buiten Roerdalslenk</t>
   </si>
   <si>
-    <t>Pleisocene afzettingen</t>
-  </si>
-  <si>
     <t>Sy</t>
   </si>
   <si>
@@ -1413,15 +1410,6 @@
     <t>yellowgreen</t>
   </si>
   <si>
-    <t>A0???</t>
-  </si>
-  <si>
-    <t>Paarse laag</t>
-  </si>
-  <si>
-    <t>Grijsgroene laag</t>
-  </si>
-  <si>
     <t>lightyellow</t>
   </si>
   <si>
@@ -1431,21 +1419,6 @@
     <t>darkgreen</t>
   </si>
   <si>
-    <t>Violette laag</t>
-  </si>
-  <si>
-    <t>Zalmkleurige laag</t>
-  </si>
-  <si>
-    <t>Bruine laag</t>
-  </si>
-  <si>
-    <t>Groene laag</t>
-  </si>
-  <si>
-    <t>Donker groene laag</t>
-  </si>
-  <si>
     <t>darkviolet</t>
   </si>
   <si>
@@ -1453,6 +1426,66 @@
   </si>
   <si>
     <t>zero-based</t>
+  </si>
+  <si>
+    <t>Pleistocene afzettingen</t>
+  </si>
+  <si>
+    <t>A0170</t>
+  </si>
+  <si>
+    <t>Onder-Oligoceen Aquifersysteem</t>
+  </si>
+  <si>
+    <t>A0450</t>
+  </si>
+  <si>
+    <t>Wemmel-Lede Aquifer</t>
+  </si>
+  <si>
+    <t>Zand van Brussel</t>
+  </si>
+  <si>
+    <t>A0610</t>
+  </si>
+  <si>
+    <t>A0620</t>
+  </si>
+  <si>
+    <t>Ieperiaan Aquitardsysteem</t>
+  </si>
+  <si>
+    <t>Landeniaan Aquifersysteem</t>
+  </si>
+  <si>
+    <t>Landeniaan en Heersiaan Aquitard</t>
+  </si>
+  <si>
+    <t>Krijt Aquifersysteem</t>
+  </si>
+  <si>
+    <t>Cambrio-Siluur Massief van Brabant</t>
+  </si>
+  <si>
+    <t>A1340</t>
+  </si>
+  <si>
+    <t>A1100</t>
+  </si>
+  <si>
+    <t>A1020</t>
+  </si>
+  <si>
+    <t>A1010</t>
+  </si>
+  <si>
+    <t>A0900</t>
+  </si>
+  <si>
+    <t>gold</t>
+  </si>
+  <si>
+    <t>COMPLEX</t>
   </si>
 </sst>
 </file>
@@ -1583,7 +1616,7 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1605,6 +1638,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -1991,7 +2025,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
@@ -3567,8 +3601,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C06500DB-BECE-8C4B-B4E6-A47BC546FCEB}">
   <dimension ref="A1:H477"/>
   <sheetViews>
-    <sheetView topLeftCell="A204" zoomScale="182" zoomScaleNormal="182" workbookViewId="0">
-      <selection activeCell="C219" sqref="C219"/>
+    <sheetView zoomScale="182" zoomScaleNormal="182" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3693,7 +3727,7 @@
         <v>110</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>382</v>
+        <v>426</v>
       </c>
       <c r="D11" s="11" t="s">
         <v>383</v>
@@ -5852,7 +5886,7 @@
         <v>45</v>
       </c>
       <c r="C218" s="11" t="s">
-        <v>414</v>
+        <v>405</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.15">
@@ -11873,7 +11907,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
-        <v>415</v>
+        <v>406</v>
       </c>
       <c r="C1" s="9"/>
       <c r="D1" s="9"/>
@@ -11933,8 +11967,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:I57"/>
   <sheetViews>
-    <sheetView zoomScale="237" zoomScaleNormal="237" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" zoomScale="237" zoomScaleNormal="237" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -11956,13 +11990,13 @@
         <v>77</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>392</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>393</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>394</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>395</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>386</v>
@@ -11976,22 +12010,22 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="C2" s="17">
         <v>5</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="17">
         <v>2</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="17">
         <v>0.15</v>
       </c>
       <c r="F2" s="2">
         <v>1E-4</v>
       </c>
       <c r="G2" s="16" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="H2" s="11" t="s">
         <v>388</v>
@@ -12005,22 +12039,22 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="C3" s="17">
         <v>10</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="17">
         <v>10</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="17">
         <v>0.2</v>
       </c>
       <c r="F3" s="2">
         <v>1E-4</v>
       </c>
       <c r="G3" s="16" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="H3" s="11" t="s">
         <v>390</v>
@@ -12034,28 +12068,28 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>0.5</v>
-      </c>
-      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="C4" s="17">
+        <v>20</v>
+      </c>
+      <c r="D4" s="17">
+        <v>10</v>
+      </c>
+      <c r="E4" s="17">
         <v>0.2</v>
-      </c>
-      <c r="E4">
-        <v>0.1</v>
       </c>
       <c r="F4" s="2">
         <v>1E-4</v>
       </c>
-      <c r="G4" s="16" t="s">
-        <v>399</v>
+      <c r="G4" s="11" t="s">
+        <v>425</v>
       </c>
       <c r="H4" s="11" t="s">
-        <v>402</v>
+        <v>408</v>
       </c>
       <c r="I4" s="11" t="s">
-        <v>403</v>
+        <v>407</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.15">
@@ -12063,28 +12097,28 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5">
-        <v>0.1</v>
-      </c>
-      <c r="D5">
-        <v>0.02</v>
-      </c>
-      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="C5" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="D5" s="17">
+        <v>0.2</v>
+      </c>
+      <c r="E5" s="17">
         <v>0.1</v>
       </c>
       <c r="F5" s="2">
         <v>1E-4</v>
       </c>
       <c r="G5" s="16" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>402</v>
+        <v>410</v>
       </c>
       <c r="I5" s="11" t="s">
-        <v>404</v>
+        <v>409</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.15">
@@ -12092,28 +12126,28 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6">
-        <v>50</v>
-      </c>
-      <c r="D6">
-        <v>25</v>
-      </c>
-      <c r="E6">
-        <v>0.25</v>
+        <v>0</v>
+      </c>
+      <c r="C6" s="17">
+        <v>0.1</v>
+      </c>
+      <c r="D6" s="17">
+        <v>0.02</v>
+      </c>
+      <c r="E6" s="17">
+        <v>0.1</v>
       </c>
       <c r="F6" s="2">
         <v>1E-4</v>
       </c>
       <c r="G6" s="16" t="s">
-        <v>396</v>
+        <v>400</v>
       </c>
       <c r="H6" s="11" t="s">
-        <v>402</v>
+        <v>413</v>
       </c>
       <c r="I6" s="11" t="s">
-        <v>392</v>
+        <v>411</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.15">
@@ -12121,28 +12155,28 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>0.1</v>
-      </c>
-      <c r="D7">
-        <v>0.03</v>
-      </c>
-      <c r="E7">
-        <v>0.1</v>
+        <v>1</v>
+      </c>
+      <c r="C7" s="17">
+        <v>20</v>
+      </c>
+      <c r="D7" s="17">
+        <v>5</v>
+      </c>
+      <c r="E7" s="17">
+        <v>0.2</v>
       </c>
       <c r="F7" s="2">
         <v>1E-4</v>
       </c>
       <c r="G7" s="16" t="s">
-        <v>413</v>
+        <v>395</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>402</v>
+        <v>414</v>
       </c>
       <c r="I7" s="11" t="s">
-        <v>408</v>
+        <v>412</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.15">
@@ -12152,26 +12186,26 @@
       <c r="B8">
         <v>0</v>
       </c>
-      <c r="C8" s="2">
-        <v>3</v>
-      </c>
-      <c r="D8" s="2">
-        <v>1</v>
-      </c>
-      <c r="E8" s="2">
+      <c r="C8" s="17">
+        <v>0.01</v>
+      </c>
+      <c r="D8" s="17">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="E8" s="17">
         <v>0.1</v>
       </c>
       <c r="F8" s="2">
         <v>1E-4</v>
       </c>
       <c r="G8" s="16" t="s">
-        <v>398</v>
+        <v>404</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>402</v>
+        <v>424</v>
       </c>
       <c r="I8" s="11" t="s">
-        <v>409</v>
+        <v>415</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.15">
@@ -12181,26 +12215,26 @@
       <c r="B9">
         <v>0</v>
       </c>
-      <c r="C9">
-        <v>0.01</v>
-      </c>
-      <c r="D9">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="E9">
+      <c r="C9" s="17">
+        <v>3</v>
+      </c>
+      <c r="D9" s="17">
+        <v>1</v>
+      </c>
+      <c r="E9" s="17">
         <v>0.1</v>
       </c>
       <c r="F9" s="2">
         <v>1E-4</v>
       </c>
       <c r="G9" s="16" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="H9" s="11" t="s">
-        <v>402</v>
+        <v>423</v>
       </c>
       <c r="I9" s="11" t="s">
-        <v>410</v>
+        <v>416</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.15">
@@ -12210,26 +12244,26 @@
       <c r="B10">
         <v>0</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="17">
         <v>0.01</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="17">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="17">
         <v>0.1</v>
       </c>
       <c r="F10" s="2">
         <v>1E-4</v>
       </c>
       <c r="G10" s="16" t="s">
-        <v>406</v>
+        <v>399</v>
       </c>
       <c r="H10" s="11" t="s">
-        <v>402</v>
+        <v>422</v>
       </c>
       <c r="I10" s="11" t="s">
-        <v>411</v>
+        <v>417</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.15">
@@ -12239,33 +12273,56 @@
       <c r="B11">
         <v>0</v>
       </c>
-      <c r="C11">
-        <v>1E-4</v>
-      </c>
-      <c r="D11">
-        <v>3.0000000000000001E-5</v>
-      </c>
-      <c r="E11">
+      <c r="C11" s="17">
+        <v>0.01</v>
+      </c>
+      <c r="D11" s="17">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="E11" s="17">
         <v>0.1</v>
       </c>
       <c r="F11" s="2">
         <v>1E-4</v>
       </c>
       <c r="G11" s="16" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="H11" s="11" t="s">
-        <v>402</v>
+        <v>421</v>
       </c>
       <c r="I11" s="11" t="s">
-        <v>412</v>
+        <v>418</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12" s="17">
+        <v>1E-4</v>
+      </c>
+      <c r="D12" s="17">
+        <v>3.0000000000000001E-5</v>
+      </c>
+      <c r="E12" s="17">
+        <v>0.1</v>
+      </c>
+      <c r="F12" s="2">
+        <v>1E-4</v>
+      </c>
+      <c r="G12" s="16" t="s">
+        <v>403</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>420</v>
+      </c>
+      <c r="I12" s="11" t="s">
+        <v>419</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.15">
       <c r="D13" s="2"/>

</xml_diff>